<commit_message>
update shop and ball
</commit_message>
<xml_diff>
--- a/excelCfg/GameData.xlsx
+++ b/excelCfg/GameData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="player" sheetId="1" r:id="rId1"/>
-    <sheet name="enemy" sheetId="2" r:id="rId2"/>
-    <sheet name="level" sheetId="3" r:id="rId3"/>
+    <sheet name="ball" sheetId="4" r:id="rId2"/>
+    <sheet name="enemy" sheetId="2" r:id="rId3"/>
+    <sheet name="level" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +137,66 @@
   </si>
   <si>
     <t>bulletSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>locked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解锁状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ffffff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ffea00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fe0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#6500ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ff5a00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ff009a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#06ff00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#0075ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>locked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜色</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -459,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,7 +532,7 @@
     <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +551,11 @@
       <c r="F1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -510,8 +574,11 @@
       <c r="F2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -530,8 +597,11 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -550,8 +620,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -570,8 +643,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -590,8 +666,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -610,8 +689,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -630,8 +712,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -650,8 +735,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -670,8 +758,11 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -690,8 +781,11 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -710,8 +804,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -730,8 +827,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -750,8 +850,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -770,8 +873,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -790,8 +896,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -810,8 +919,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -830,8 +942,11 @@
       <c r="F18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -850,8 +965,11 @@
       <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -870,8 +988,11 @@
       <c r="F20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
@@ -890,8 +1011,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
@@ -910,8 +1034,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -930,8 +1057,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -950,8 +1080,11 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -970,8 +1103,11 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -990,8 +1126,11 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1010,8 +1149,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1030,8 +1172,11 @@
       <c r="F28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1050,8 +1195,11 @@
       <c r="F29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1070,8 +1218,11 @@
       <c r="F30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1090,8 +1241,11 @@
       <c r="F31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1110,8 +1264,11 @@
       <c r="F32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1130,8 +1287,11 @@
       <c r="F33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1149,6 +1309,9 @@
       </c>
       <c r="F34">
         <v>3</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1158,6 +1321,176 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1257,7 +1590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>

</xml_diff>

<commit_message>
update level and enemy type
</commit_message>
<xml_diff>
--- a/excelCfg/GameData.xlsx
+++ b/excelCfg/GameData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="player" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="ball" sheetId="4" r:id="rId3"/>
     <sheet name="reward" sheetId="5" r:id="rId4"/>
     <sheet name="enemy" sheetId="2" r:id="rId5"/>
-    <sheet name="type4" sheetId="7" r:id="rId6"/>
-    <sheet name="level" sheetId="3" r:id="rId7"/>
+    <sheet name="level" sheetId="3" r:id="rId6"/>
+    <sheet name="type4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -2311,10 +2311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,7 +2386,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2414,6 +2414,20 @@
         <v>8</v>
       </c>
       <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
     </row>
@@ -2425,210 +2439,124 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2639,124 +2567,210 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>